<commit_message>
#33 added macros in process.h
</commit_message>
<xml_diff>
--- a/eOS/Documentation/eOS V2 process state field.xlsx
+++ b/eOS/Documentation/eOS V2 process state field.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>8&lt;-&gt;15</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Task Id</t>
+  </si>
+  <si>
+    <t>Validity</t>
+  </si>
+  <si>
+    <t>0=invalid</t>
+  </si>
+  <si>
+    <t>1=valid</t>
   </si>
 </sst>
 </file>
@@ -447,7 +456,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +517,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -533,8 +542,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -548,8 +557,14 @@
       <c r="F4" t="s">
         <v>27</v>
       </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
#33 Removed Medium Prio. A task will have only 2 priorities: High and Low
</commit_message>
<xml_diff>
--- a/eOS/Documentation/eOS V2 process state field.xlsx
+++ b/eOS/Documentation/eOS V2 process state field.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>8&lt;-&gt;15</t>
   </si>
@@ -89,12 +89,6 @@
     <t>00=High</t>
   </si>
   <si>
-    <t>01=Medium</t>
-  </si>
-  <si>
-    <t>10=Low</t>
-  </si>
-  <si>
     <t>11=Not Used</t>
   </si>
   <si>
@@ -129,6 +123,9 @@
   </si>
   <si>
     <t>1=valid</t>
+  </si>
+  <si>
+    <t>01=Low</t>
   </si>
 </sst>
 </file>
@@ -456,7 +453,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -535,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -543,7 +540,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -552,10 +549,10 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -563,19 +560,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -583,27 +580,27 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>